<commit_message>
Included sample wireframe in layout worksheet
</commit_message>
<xml_diff>
--- a/frontend/AttendanceProject.xlsx
+++ b/frontend/AttendanceProject.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Objective" sheetId="1" state="visible" r:id="rId3"/>
@@ -405,6 +405,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514440</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>631800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>56520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3585960" y="678600"/>
+          <a:ext cx="1742760" cy="2466720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
@@ -518,7 +561,7 @@
   </sheetPr>
   <dimension ref="B2:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -959,8 +1002,8 @@
   </sheetPr>
   <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1001,5 +1044,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>